<commit_message>
Không biết gì hết
</commit_message>
<xml_diff>
--- a/Private/Phương/4. Timelog/PM_TimeLog_Phương.xlsx
+++ b/Private/Phương/4. Timelog/PM_TimeLog_Phương.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\GitHub\Capstone-Project\Private\Phương\4. Timelog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AB5E127-255F-48DC-9A37-257999611249}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{205BEE36-E8FB-4AC3-8A80-988EA01D2D18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="99">
   <si>
     <t>Work in period</t>
   </si>
@@ -325,14 +325,28 @@
   </si>
   <si>
     <t xml:space="preserve">Research React </t>
+  </si>
+  <si>
+    <t>28/10/2019</t>
+  </si>
+  <si>
+    <t>29/10/2019</t>
+  </si>
+  <si>
+    <t>30/10/2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Research GIS , 
+prepare question for customer </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-1010000]d/m/yy;@"/>
+    <numFmt numFmtId="167" formatCode="mm/dd/yyyy;@"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -868,7 +882,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1062,6 +1076,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -4581,8 +4601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40E6E6FC-AA3E-4AB8-932A-DA22E440EB21}">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4591,7 +4611,7 @@
     <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="40.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5036,7 +5056,7 @@
       </c>
       <c r="I19" s="77"/>
     </row>
-    <row r="20" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="12">
         <v>3</v>
       </c>
@@ -5046,11 +5066,11 @@
       <c r="C20" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="66" t="s">
-        <v>94</v>
+      <c r="D20" s="79" t="s">
+        <v>98</v>
       </c>
       <c r="E20" s="22" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="F20" s="12">
         <v>5.5</v>
@@ -5063,7 +5083,7 @@
       </c>
       <c r="I20" s="19"/>
     </row>
-    <row r="21" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="12">
         <v>3</v>
       </c>
@@ -5074,21 +5094,21 @@
         <v>63</v>
       </c>
       <c r="D21" s="66"/>
-      <c r="E21" s="23" t="s">
-        <v>72</v>
+      <c r="E21" s="22" t="s">
+        <v>96</v>
       </c>
       <c r="F21" s="12">
         <v>4</v>
       </c>
       <c r="G21" s="12">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H21" s="18" t="s">
         <v>20</v>
       </c>
       <c r="I21" s="19"/>
     </row>
-    <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="12">
         <v>3</v>
       </c>
@@ -5099,11 +5119,11 @@
         <v>61</v>
       </c>
       <c r="D22" s="67"/>
-      <c r="E22" s="21" t="s">
-        <v>73</v>
+      <c r="E22" s="22" t="s">
+        <v>97</v>
       </c>
       <c r="F22" s="1">
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="G22" s="1">
         <v>5</v>
@@ -5113,7 +5133,7 @@
       </c>
       <c r="I22" s="3"/>
     </row>
-    <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="12">
         <v>3</v>
       </c>
@@ -5126,21 +5146,21 @@
       <c r="D23" s="67" t="s">
         <v>93</v>
       </c>
-      <c r="E23" s="23" t="s">
-        <v>74</v>
+      <c r="E23" s="78">
+        <v>43476</v>
       </c>
       <c r="F23" s="1">
         <v>5</v>
       </c>
       <c r="G23" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H23" s="18" t="s">
         <v>20</v>
       </c>
       <c r="I23" s="3"/>
     </row>
-    <row r="24" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="12">
         <v>3</v>
       </c>
@@ -5153,8 +5173,8 @@
       <c r="D24" s="67" t="s">
         <v>94</v>
       </c>
-      <c r="E24" s="20" t="s">
-        <v>77</v>
+      <c r="E24" s="78">
+        <v>43507</v>
       </c>
       <c r="F24" s="1">
         <v>4.5</v>
@@ -5180,14 +5200,14 @@
       <c r="D25" s="69" t="s">
         <v>92</v>
       </c>
-      <c r="E25" s="20" t="s">
-        <v>91</v>
+      <c r="E25" s="78">
+        <v>43535</v>
       </c>
       <c r="F25" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G25" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H25" s="18" t="s">
         <v>20</v>
@@ -5214,7 +5234,7 @@
       </c>
       <c r="C27" s="76">
         <f>SUM(F20:F26)</f>
-        <v>27</v>
+        <v>29.5</v>
       </c>
       <c r="D27" s="76"/>
       <c r="E27" s="76"/>
@@ -5224,7 +5244,7 @@
       </c>
       <c r="H27" s="76">
         <f>SUM(G20:G26)</f>
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I27" s="77"/>
     </row>
@@ -5238,6 +5258,7 @@
     <mergeCell ref="C19:F19"/>
     <mergeCell ref="H19:I19"/>
   </mergeCells>
+  <phoneticPr fontId="8" type="noConversion"/>
   <dataValidations count="4">
     <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{E33165A0-C84D-4A86-B33D-34CB51D1AC5F}">
       <formula1>B4</formula1>
@@ -5254,5 +5275,6 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
bien ban kh , timelog
</commit_message>
<xml_diff>
--- a/Private/Phương/4. Timelog/PM_TimeLog_Phương.xlsx
+++ b/Private/Phương/4. Timelog/PM_TimeLog_Phương.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\GitHub\Capstone-Project\Private\Phương\4. Timelog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{205BEE36-E8FB-4AC3-8A80-988EA01D2D18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91D9B36A-242C-40EE-914F-7FF580887A6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="111">
   <si>
     <t>Work in period</t>
   </si>
@@ -336,8 +336,48 @@
     <t>30/10/2019</t>
   </si>
   <si>
+    <t>31/10/2019</t>
+  </si>
+  <si>
+    <t>Test Process</t>
+  </si>
+  <si>
+    <t>Requiment process</t>
+  </si>
+  <si>
     <t xml:space="preserve">Research GIS , 
-prepare question for customer </t>
+prepare question for customer 
+Test plan </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Requiment plan </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Complete the meeting minutes ; 
+Review document ,  test process </t>
+  </si>
+  <si>
+    <t>TE_Testprocess_ver1.0</t>
+  </si>
+  <si>
+    <t>RE_RequimentPlan_ver1.0</t>
+  </si>
+  <si>
+    <t>RE_RequimentProcess_ver1.0</t>
+  </si>
+  <si>
+    <t>TE_Testplan_ver1.0</t>
+  </si>
+  <si>
+    <t>Meeting_Customer_29/10/2019
+Meeting_Mentor _30/10/2019</t>
+  </si>
+  <si>
+    <t>Meeting_Mentor_14/10/2019
+Meeting-customer_18/10/2019</t>
+  </si>
+  <si>
+    <t>Meeting_Mentor_23/10/2019</t>
   </si>
 </sst>
 </file>
@@ -346,7 +386,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-1010000]d/m/yy;@"/>
-    <numFmt numFmtId="167" formatCode="mm/dd/yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="mm/dd/yyyy;@"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -882,7 +922,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1053,6 +1093,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1077,11 +1123,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -4154,17 +4197,17 @@
       <c r="I1" s="26"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="72" t="s">
+      <c r="A2" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="73"/>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="74"/>
-      <c r="H2" s="74"/>
-      <c r="I2" s="75"/>
+      <c r="B2" s="75"/>
+      <c r="C2" s="76"/>
+      <c r="D2" s="76"/>
+      <c r="E2" s="76"/>
+      <c r="F2" s="76"/>
+      <c r="G2" s="76"/>
+      <c r="H2" s="76"/>
+      <c r="I2" s="77"/>
     </row>
     <row r="3" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
@@ -4364,21 +4407,21 @@
       <c r="B11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="70">
+      <c r="C11" s="72">
         <f>SUM(F4:F10)</f>
         <v>24</v>
       </c>
-      <c r="D11" s="70"/>
-      <c r="E11" s="70"/>
-      <c r="F11" s="71"/>
+      <c r="D11" s="72"/>
+      <c r="E11" s="72"/>
+      <c r="F11" s="73"/>
       <c r="G11" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H11" s="70">
+      <c r="H11" s="72">
         <f>SUM(G4:G10)</f>
         <v>24</v>
       </c>
-      <c r="I11" s="71"/>
+      <c r="I11" s="73"/>
     </row>
     <row r="12" spans="1:11" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A12" s="12">
@@ -4552,21 +4595,21 @@
       <c r="B19" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="70">
+      <c r="C19" s="72">
         <f>SUM(F12:F18)</f>
         <v>22</v>
       </c>
-      <c r="D19" s="70"/>
-      <c r="E19" s="70"/>
-      <c r="F19" s="71"/>
+      <c r="D19" s="72"/>
+      <c r="E19" s="72"/>
+      <c r="F19" s="73"/>
       <c r="G19" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H19" s="70">
+      <c r="H19" s="72">
         <f>SUM(G12:G18)</f>
         <v>34</v>
       </c>
-      <c r="I19" s="71"/>
+      <c r="I19" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -4599,10 +4642,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40E6E6FC-AA3E-4AB8-932A-DA22E440EB21}">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4612,7 +4655,8 @@
     <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="40.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" customWidth="1"/>
+    <col min="9" max="9" width="32.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4629,17 +4673,17 @@
       <c r="I1" s="26"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="72" t="s">
+      <c r="A2" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="73"/>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="74"/>
-      <c r="H2" s="74"/>
-      <c r="I2" s="75"/>
+      <c r="B2" s="75"/>
+      <c r="C2" s="76"/>
+      <c r="D2" s="76"/>
+      <c r="E2" s="76"/>
+      <c r="F2" s="76"/>
+      <c r="G2" s="76"/>
+      <c r="H2" s="76"/>
+      <c r="I2" s="77"/>
     </row>
     <row r="3" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
@@ -4801,7 +4845,7 @@
       </c>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>1</v>
       </c>
@@ -4826,7 +4870,9 @@
       <c r="H9" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="I9" s="3"/>
+      <c r="I9" s="80" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="10" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11"/>
@@ -4846,21 +4892,21 @@
       <c r="B11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="76">
+      <c r="C11" s="78">
         <f>SUM(F4:F10)</f>
         <v>27</v>
       </c>
-      <c r="D11" s="76"/>
-      <c r="E11" s="76"/>
-      <c r="F11" s="77"/>
+      <c r="D11" s="78"/>
+      <c r="E11" s="78"/>
+      <c r="F11" s="79"/>
       <c r="G11" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H11" s="76">
+      <c r="H11" s="78">
         <f>SUM(G4:G10)</f>
         <v>30</v>
       </c>
-      <c r="I11" s="77"/>
+      <c r="I11" s="79"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
@@ -5020,7 +5066,9 @@
       <c r="H17" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="I17" s="3"/>
+      <c r="I17" s="3" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="18" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="11"/>
@@ -5040,23 +5088,23 @@
       <c r="B19" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="76">
+      <c r="C19" s="78">
         <f>SUM(F12:F18)</f>
         <v>29</v>
       </c>
-      <c r="D19" s="76"/>
-      <c r="E19" s="76"/>
-      <c r="F19" s="77"/>
+      <c r="D19" s="78"/>
+      <c r="E19" s="78"/>
+      <c r="F19" s="79"/>
       <c r="G19" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H19" s="76">
+      <c r="H19" s="78">
         <f>SUM(G12:G18)</f>
         <v>30</v>
       </c>
-      <c r="I19" s="77"/>
-    </row>
-    <row r="20" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I19" s="79"/>
+    </row>
+    <row r="20" spans="1:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="12">
         <v>3</v>
       </c>
@@ -5066,8 +5114,8 @@
       <c r="C20" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="79" t="s">
-        <v>98</v>
+      <c r="D20" s="71" t="s">
+        <v>101</v>
       </c>
       <c r="E20" s="22" t="s">
         <v>95</v>
@@ -5079,7 +5127,7 @@
         <v>6</v>
       </c>
       <c r="H20" s="18" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I20" s="19"/>
     </row>
@@ -5146,8 +5194,8 @@
       <c r="D23" s="67" t="s">
         <v>93</v>
       </c>
-      <c r="E23" s="78">
-        <v>43476</v>
+      <c r="E23" s="70" t="s">
+        <v>98</v>
       </c>
       <c r="F23" s="1">
         <v>5</v>
@@ -5158,7 +5206,9 @@
       <c r="H23" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="I23" s="3"/>
+      <c r="I23" s="3" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="24" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="12">
@@ -5173,8 +5223,8 @@
       <c r="D24" s="67" t="s">
         <v>94</v>
       </c>
-      <c r="E24" s="78">
-        <v>43507</v>
+      <c r="E24" s="70">
+        <v>43476</v>
       </c>
       <c r="F24" s="1">
         <v>4.5</v>
@@ -5187,7 +5237,7 @@
       </c>
       <c r="I24" s="3"/>
     </row>
-    <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
         <v>3</v>
       </c>
@@ -5200,8 +5250,8 @@
       <c r="D25" s="69" t="s">
         <v>92</v>
       </c>
-      <c r="E25" s="78">
-        <v>43535</v>
+      <c r="E25" s="70">
+        <v>43507</v>
       </c>
       <c r="F25" s="1">
         <v>6</v>
@@ -5210,9 +5260,11 @@
         <v>7</v>
       </c>
       <c r="H25" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="I25" s="3"/>
+        <v>21</v>
+      </c>
+      <c r="I25" s="80" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="26" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="11"/>
@@ -5232,24 +5284,224 @@
       <c r="B27" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C27" s="76">
+      <c r="C27" s="78">
         <f>SUM(F20:F26)</f>
         <v>29.5</v>
       </c>
-      <c r="D27" s="76"/>
-      <c r="E27" s="76"/>
-      <c r="F27" s="77"/>
+      <c r="D27" s="78"/>
+      <c r="E27" s="78"/>
+      <c r="F27" s="79"/>
       <c r="G27" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H27" s="76">
+      <c r="H27" s="78">
         <f>SUM(G20:G26)</f>
         <v>35</v>
       </c>
-      <c r="I27" s="77"/>
+      <c r="I27" s="79"/>
+    </row>
+    <row r="28" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="12">
+        <v>4</v>
+      </c>
+      <c r="B28" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="D28" s="71" t="s">
+        <v>102</v>
+      </c>
+      <c r="E28" s="22">
+        <v>43773</v>
+      </c>
+      <c r="F28" s="12">
+        <v>5.5</v>
+      </c>
+      <c r="G28" s="12">
+        <v>7</v>
+      </c>
+      <c r="H28" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="I28" s="19" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="12">
+        <v>4</v>
+      </c>
+      <c r="B29" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="D29" s="66" t="s">
+        <v>100</v>
+      </c>
+      <c r="E29" s="22">
+        <v>43774</v>
+      </c>
+      <c r="F29" s="12">
+        <v>5</v>
+      </c>
+      <c r="G29" s="12">
+        <v>6</v>
+      </c>
+      <c r="H29" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="I29" s="19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="12">
+        <v>4</v>
+      </c>
+      <c r="B30" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="D30" s="67"/>
+      <c r="E30" s="22">
+        <v>43775</v>
+      </c>
+      <c r="F30" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="G30" s="1">
+        <v>5</v>
+      </c>
+      <c r="H30" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="I30" s="3"/>
+    </row>
+    <row r="31" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="12">
+        <v>4</v>
+      </c>
+      <c r="B31" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="D31" s="67" t="s">
+        <v>99</v>
+      </c>
+      <c r="E31" s="22">
+        <v>43776</v>
+      </c>
+      <c r="F31" s="1">
+        <v>5</v>
+      </c>
+      <c r="G31" s="1">
+        <v>7</v>
+      </c>
+      <c r="H31" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="I31" s="3"/>
+    </row>
+    <row r="32" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="12">
+        <v>4</v>
+      </c>
+      <c r="B32" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="D32" s="67"/>
+      <c r="E32" s="22">
+        <v>43777</v>
+      </c>
+      <c r="F32" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="G32" s="1">
+        <v>5</v>
+      </c>
+      <c r="H32" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="I32" s="3"/>
+    </row>
+    <row r="33" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="12">
+        <v>4</v>
+      </c>
+      <c r="B33" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="D33" s="69" t="s">
+        <v>103</v>
+      </c>
+      <c r="E33" s="22">
+        <v>43778</v>
+      </c>
+      <c r="F33" s="1">
+        <v>7</v>
+      </c>
+      <c r="G33" s="1">
+        <v>5</v>
+      </c>
+      <c r="H33" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="11"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="68"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="18"/>
+      <c r="I34" s="5"/>
+    </row>
+    <row r="35" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C35" s="78">
+        <f>SUM(F28:F34)</f>
+        <v>31.5</v>
+      </c>
+      <c r="D35" s="78"/>
+      <c r="E35" s="78"/>
+      <c r="F35" s="79"/>
+      <c r="G35" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H35" s="78">
+        <f>SUM(G28:G34)</f>
+        <v>35</v>
+      </c>
+      <c r="I35" s="79"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="9">
+    <mergeCell ref="C35:F35"/>
+    <mergeCell ref="H35:I35"/>
     <mergeCell ref="C27:F27"/>
     <mergeCell ref="H27:I27"/>
     <mergeCell ref="A2:I2"/>
@@ -5264,13 +5516,13 @@
       <formula1>B4</formula1>
       <formula2>B10</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4:H10 H12:H18 H20:H26" xr:uid="{72DA7AFC-686F-4552-A46C-54827227E2DF}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4:H10 H12:H18 H20:H26 H28:H34" xr:uid="{72DA7AFC-686F-4552-A46C-54827227E2DF}">
       <formula1>"Done,Inprogress "</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C9 C12:C17 C20:C25" xr:uid="{CA2FE6F4-962B-45C9-BD0E-B095FA55B23A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C9 C12:C17 C20:C25 C28:C33" xr:uid="{CA2FE6F4-962B-45C9-BD0E-B095FA55B23A}">
       <formula1>"Project Management, Requirement, Architecture and Desgin, Implementation, Testing, Training, Meetting Customer, Meeting Mentor"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10 C18 C26" xr:uid="{ED2FDDC9-5592-49AD-9E51-6F9CA9FF49FF}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10 C18 C26 C34" xr:uid="{ED2FDDC9-5592-49AD-9E51-6F9CA9FF49FF}">
       <formula1>"Project Management, Requirement, Architecture and Desgin, Implementation, Testing, Training, Meetting Customer, Meetting Mentor"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
UCD - Proccess RE
</commit_message>
<xml_diff>
--- a/Private/Phương/4. Timelog/PM_TimeLog_Phương.xlsx
+++ b/Private/Phương/4. Timelog/PM_TimeLog_Phương.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\GitHub\Capstone-Project\Private\Phương\4. Timelog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91D9B36A-242C-40EE-914F-7FF580887A6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FC77334-21A1-4E79-AA93-E376CF75E792}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="113">
   <si>
     <t>Work in period</t>
   </si>
@@ -378,6 +378,14 @@
   </si>
   <si>
     <t>Meeting_Mentor_23/10/2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Complete the meeting minutes ;
+Review document </t>
+  </si>
+  <si>
+    <t>Meeting_customer 8/10/2019
+Meeting_mentor 6/10/2019</t>
   </si>
 </sst>
 </file>
@@ -4642,10 +4650,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40E6E6FC-AA3E-4AB8-932A-DA22E440EB21}">
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5458,7 +5466,7 @@
         <v>5</v>
       </c>
       <c r="H33" s="18" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I33" s="3" t="s">
         <v>104</v>
@@ -5498,10 +5506,200 @@
       </c>
       <c r="I35" s="79"/>
     </row>
+    <row r="36" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="12">
+        <v>4</v>
+      </c>
+      <c r="B36" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="C36" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="D36" s="71" t="s">
+        <v>111</v>
+      </c>
+      <c r="E36" s="22">
+        <v>43773</v>
+      </c>
+      <c r="F36" s="12">
+        <v>5.5</v>
+      </c>
+      <c r="G36" s="12">
+        <v>5</v>
+      </c>
+      <c r="H36" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="I36" s="19" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="12">
+        <v>4</v>
+      </c>
+      <c r="B37" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="C37" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="D37" s="66"/>
+      <c r="E37" s="22">
+        <v>43774</v>
+      </c>
+      <c r="F37" s="12">
+        <v>5</v>
+      </c>
+      <c r="G37" s="12">
+        <v>6</v>
+      </c>
+      <c r="H37" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="I37" s="19"/>
+    </row>
+    <row r="38" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="12">
+        <v>4</v>
+      </c>
+      <c r="B38" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="D38" s="67"/>
+      <c r="E38" s="22">
+        <v>43775</v>
+      </c>
+      <c r="F38" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="G38" s="1">
+        <v>5</v>
+      </c>
+      <c r="H38" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="I38" s="3"/>
+    </row>
+    <row r="39" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="12">
+        <v>4</v>
+      </c>
+      <c r="B39" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="C39" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="D39" s="67"/>
+      <c r="E39" s="22">
+        <v>43776</v>
+      </c>
+      <c r="F39" s="1">
+        <v>5</v>
+      </c>
+      <c r="G39" s="1">
+        <v>7</v>
+      </c>
+      <c r="H39" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="I39" s="3"/>
+    </row>
+    <row r="40" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="12">
+        <v>4</v>
+      </c>
+      <c r="B40" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="C40" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="D40" s="67"/>
+      <c r="E40" s="22">
+        <v>43777</v>
+      </c>
+      <c r="F40" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="G40" s="1">
+        <v>5</v>
+      </c>
+      <c r="H40" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="I40" s="3"/>
+    </row>
+    <row r="41" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="12">
+        <v>4</v>
+      </c>
+      <c r="B41" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="C41" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="D41" s="69"/>
+      <c r="E41" s="22">
+        <v>43778</v>
+      </c>
+      <c r="F41" s="1">
+        <v>7</v>
+      </c>
+      <c r="G41" s="1">
+        <v>5</v>
+      </c>
+      <c r="H41" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="I41" s="3"/>
+    </row>
+    <row r="42" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="11"/>
+      <c r="B42" s="13"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="68"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="11"/>
+      <c r="G42" s="11"/>
+      <c r="H42" s="18"/>
+      <c r="I42" s="5"/>
+    </row>
+    <row r="43" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C43" s="78">
+        <f>SUM(F36:F42)</f>
+        <v>31.5</v>
+      </c>
+      <c r="D43" s="78"/>
+      <c r="E43" s="78"/>
+      <c r="F43" s="79"/>
+      <c r="G43" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H43" s="78">
+        <f>SUM(G36:G42)</f>
+        <v>33</v>
+      </c>
+      <c r="I43" s="79"/>
+    </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="11">
     <mergeCell ref="C35:F35"/>
     <mergeCell ref="H35:I35"/>
+    <mergeCell ref="C43:F43"/>
+    <mergeCell ref="H43:I43"/>
     <mergeCell ref="C27:F27"/>
     <mergeCell ref="H27:I27"/>
     <mergeCell ref="A2:I2"/>
@@ -5516,13 +5714,13 @@
       <formula1>B4</formula1>
       <formula2>B10</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4:H10 H12:H18 H20:H26 H28:H34" xr:uid="{72DA7AFC-686F-4552-A46C-54827227E2DF}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4:H10 H12:H18 H20:H26 H28:H34 H36:H42" xr:uid="{72DA7AFC-686F-4552-A46C-54827227E2DF}">
       <formula1>"Done,Inprogress "</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C9 C12:C17 C20:C25 C28:C33" xr:uid="{CA2FE6F4-962B-45C9-BD0E-B095FA55B23A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C9 C12:C17 C20:C25 C28:C33 C36:C41" xr:uid="{CA2FE6F4-962B-45C9-BD0E-B095FA55B23A}">
       <formula1>"Project Management, Requirement, Architecture and Desgin, Implementation, Testing, Training, Meetting Customer, Meeting Mentor"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10 C18 C26 C34" xr:uid="{ED2FDDC9-5592-49AD-9E51-6F9CA9FF49FF}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10 C18 C26 C34 C42" xr:uid="{ED2FDDC9-5592-49AD-9E51-6F9CA9FF49FF}">
       <formula1>"Project Management, Requirement, Architecture and Desgin, Implementation, Testing, Training, Meetting Customer, Meetting Mentor"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>